<commit_message>
Implementiing Signature on Settings and Add Reports
</commit_message>
<xml_diff>
--- a/ProgramPartListWeb/Content/Uploads/PGFY-00031FORM_1.xlsx
+++ b/ProgramPartListWeb/Content/Uploads/PGFY-00031FORM_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllSystems\P1saproject\ProgramPartListWeb\Content\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680E8767-24BE-4B62-A008-185B07D8B600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39E2CBB-D0B3-4371-B66A-0011A633299D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFE99378-DD6B-4ABB-94CE-EAE1FDD2D083}"/>
   </bookViews>
@@ -1371,6 +1371,70 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>189140</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>619125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>721880</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>273506</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="SignaImage">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBA8184F-9E8A-7BDE-8581-817D286C5F87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7809140" y="18907125"/>
+          <a:ext cx="532740" cy="359231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-PH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4300,8 +4364,8 @@
   </sheetPr>
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A41" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49:G49"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A38" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
MSD Fix Scan Quantity
</commit_message>
<xml_diff>
--- a/ProgramPartListWeb/Content/Uploads/PGFY-00031FORM_1.xlsx
+++ b/ProgramPartListWeb/Content/Uploads/PGFY-00031FORM_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllSystems\P1saproject\ProgramPartListWeb\Content\Uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.29.3.141\c$\inetpub\wwwroot\program-partlist\Content\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62680D3-38D3-49FE-9902-FF75140B22FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A318896-5644-4F7B-93C9-D94323367D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFE99378-DD6B-4ABB-94CE-EAE1FDD2D083}"/>
   </bookViews>
@@ -642,7 +642,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -764,18 +764,48 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -803,67 +833,43 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -913,8 +919,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8244111" y="244928"/>
-          <a:ext cx="5012871" cy="895350"/>
+          <a:off x="8228236" y="216353"/>
+          <a:ext cx="5012871" cy="1133475"/>
           <a:chOff x="8590186" y="149679"/>
           <a:chExt cx="4540703" cy="1340303"/>
         </a:xfrm>
@@ -4343,10 +4349,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3EFCFA-79D8-4EF9-BB37-3D635928219F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4362,7 +4371,7 @@
     <col min="9" max="9" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="39"/>
@@ -4370,17 +4379,17 @@
       <c r="F1" s="39"/>
       <c r="G1" s="40"/>
     </row>
-    <row r="2" spans="2:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+    <row r="2" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="65"/>
+      <c r="C2" s="55"/>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
       <c r="F2" s="41"/>
       <c r="G2" s="42"/>
     </row>
-    <row r="3" spans="2:9" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -4390,95 +4399,95 @@
       <c r="F3" s="41"/>
       <c r="G3" s="42"/>
     </row>
-    <row r="4" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B4" s="67" t="s">
+    <row r="4" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="68"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="43"/>
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
       <c r="G4" s="44"/>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="2:9" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="62" t="s">
+    <row r="6" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="50" t="s">
+      <c r="C6" s="59"/>
+      <c r="D6" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="52"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="55"/>
+    <row r="7" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="79"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="65"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="55"/>
+    <row r="8" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="65"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
+    <row r="9" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55"/>
+    <row r="10" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="65"/>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
+    <row r="11" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="61" t="s">
+    <row r="12" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="61"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="45" t="s">
         <v>21</v>
       </c>
@@ -4487,65 +4496,65 @@
       <c r="G12" s="45"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
+    <row r="13" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
       <c r="F13" s="45"/>
       <c r="G13" s="45"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
+    <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
       <c r="G14" s="45"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
+    <row r="15" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
       <c r="F15" s="45"/>
       <c r="G15" s="45"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
+    <row r="16" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
       <c r="F16" s="45"/>
       <c r="G16" s="45"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
+    <row r="17" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
       <c r="F17" s="45"/>
       <c r="G17" s="45"/>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
+    <row r="18" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
       <c r="F18" s="45"/>
       <c r="G18" s="45"/>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="61" t="s">
+    <row r="19" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="61"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="45" t="s">
         <v>22</v>
       </c>
@@ -4554,132 +4563,132 @@
       <c r="G19" s="45"/>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
+    <row r="20" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
       <c r="F20" s="45"/>
       <c r="G20" s="45"/>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
+    <row r="21" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45"/>
       <c r="G21" s="45"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
+    <row r="22" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
       <c r="F22" s="45"/>
       <c r="G22" s="45"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
+    <row r="23" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
       <c r="F23" s="45"/>
       <c r="G23" s="45"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
+    <row r="24" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45"/>
       <c r="G24" s="45"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
+    <row r="25" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
       <c r="F25" s="45"/>
       <c r="G25" s="45"/>
       <c r="I25" s="12"/>
     </row>
-    <row r="26" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="62" t="s">
+    <row r="26" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="62"/>
+      <c r="C26" s="59"/>
       <c r="D26" s="45"/>
       <c r="E26" s="45"/>
       <c r="F26" s="45"/>
       <c r="G26" s="45"/>
       <c r="I26" s="12"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="63" t="s">
+    <row r="27" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="63"/>
+      <c r="C27" s="79"/>
       <c r="D27" s="45"/>
       <c r="E27" s="45"/>
       <c r="F27" s="45"/>
       <c r="G27" s="45"/>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
+    <row r="28" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
       <c r="F28" s="45"/>
       <c r="G28" s="45"/>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
+    <row r="29" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
       <c r="F29" s="45"/>
       <c r="G29" s="45"/>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
+    <row r="30" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
       <c r="F30" s="45"/>
       <c r="G30" s="45"/>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
+    <row r="31" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="78"/>
+      <c r="C31" s="78"/>
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
       <c r="F31" s="45"/>
       <c r="G31" s="45"/>
       <c r="I31" s="12"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
+    <row r="32" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="78"/>
+      <c r="C32" s="78"/>
       <c r="D32" s="45"/>
       <c r="E32" s="45"/>
       <c r="F32" s="45"/>
       <c r="G32" s="45"/>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="61" t="s">
+    <row r="33" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="61"/>
+      <c r="C33" s="48"/>
       <c r="D33" s="45" t="s">
         <v>24</v>
       </c>
@@ -4688,74 +4697,74 @@
       <c r="G33" s="45"/>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
+    <row r="34" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
       <c r="F34" s="45"/>
       <c r="G34" s="45"/>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
+    <row r="35" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="78"/>
+      <c r="C35" s="78"/>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
       <c r="F35" s="45"/>
       <c r="G35" s="45"/>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
+    <row r="36" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="78"/>
+      <c r="C36" s="78"/>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
       <c r="F36" s="45"/>
       <c r="G36" s="45"/>
       <c r="I36" s="12"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
+    <row r="37" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="78"/>
+      <c r="C37" s="78"/>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
       <c r="F37" s="45"/>
       <c r="G37" s="45"/>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="60"/>
-      <c r="C38" s="60"/>
+    <row r="38" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="78"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
       <c r="F38" s="45"/>
       <c r="G38" s="45"/>
       <c r="I38" s="12"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
+    <row r="39" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="78"/>
+      <c r="C39" s="78"/>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
       <c r="F39" s="45"/>
       <c r="G39" s="45"/>
       <c r="I39" s="12"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="60"/>
-      <c r="C40" s="60"/>
+    <row r="40" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="78"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
       <c r="F40" s="45"/>
       <c r="G40" s="45"/>
       <c r="I40" s="12"/>
     </row>
-    <row r="41" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="61" t="s">
+    <row r="41" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="61"/>
+      <c r="C41" s="48"/>
       <c r="D41" s="45" t="s">
         <v>23</v>
       </c>
@@ -4764,89 +4773,89 @@
       <c r="G41" s="45"/>
       <c r="I41" s="12"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
+    <row r="42" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="77"/>
+      <c r="C42" s="77"/>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
       <c r="F42" s="45"/>
       <c r="G42" s="45"/>
       <c r="I42" s="12"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
+    <row r="43" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="78"/>
+      <c r="C43" s="78"/>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
       <c r="F43" s="45"/>
       <c r="G43" s="45"/>
       <c r="I43" s="12"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="60"/>
-      <c r="C44" s="60"/>
+    <row r="44" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="78"/>
+      <c r="C44" s="78"/>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
       <c r="F44" s="45"/>
       <c r="G44" s="45"/>
       <c r="I44" s="12"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
+    <row r="45" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="78"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
       <c r="I45" s="12"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
+    <row r="46" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="78"/>
+      <c r="C46" s="78"/>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
       <c r="F46" s="45"/>
       <c r="G46" s="45"/>
       <c r="I46" s="12"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
+    <row r="47" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="78"/>
+      <c r="C47" s="78"/>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="45"/>
       <c r="G47" s="45"/>
       <c r="I47" s="12"/>
     </row>
-    <row r="48" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="69" t="s">
+    <row r="48" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="72" t="s">
+      <c r="C48" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="75" t="s">
+      <c r="D48" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="76"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="77"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="71"/>
       <c r="I48" s="12"/>
     </row>
-    <row r="49" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="70"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="74" t="s">
+    <row r="49" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="51"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
       <c r="I49" s="12"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="70"/>
-      <c r="C50" s="72"/>
+    <row r="50" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="51"/>
+      <c r="C50" s="53"/>
       <c r="D50" s="73" t="s">
         <v>16</v>
       </c>
@@ -4855,26 +4864,26 @@
       <c r="G50" s="73"/>
       <c r="I50" s="12"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="70"/>
-      <c r="C51" s="72"/>
+    <row r="51" spans="2:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="51"/>
+      <c r="C51" s="53"/>
       <c r="D51" s="73"/>
       <c r="E51" s="73"/>
       <c r="F51" s="73"/>
       <c r="G51" s="73"/>
       <c r="I51" s="12"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="70"/>
-      <c r="C52" s="72"/>
+    <row r="52" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="51"/>
+      <c r="C52" s="53"/>
       <c r="D52" s="73"/>
       <c r="E52" s="73"/>
       <c r="F52" s="73"/>
       <c r="G52" s="73"/>
       <c r="I52" s="12"/>
     </row>
-    <row r="53" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="71"/>
+    <row r="53" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="52"/>
       <c r="C53" s="35" t="s">
         <v>19</v>
       </c>
@@ -4888,15 +4897,15 @@
       <c r="G53" s="37"/>
       <c r="I53" s="12"/>
     </row>
-    <row r="54" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="27"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="48"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="75"/>
+      <c r="F54" s="75"/>
+      <c r="G54" s="76"/>
       <c r="I54" s="19"/>
     </row>
     <row r="55" spans="2:9" ht="20.25" x14ac:dyDescent="0.25">
@@ -4985,8 +4994,8 @@
       <c r="D67" s="14"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="66"/>
-      <c r="C68" s="66"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="14"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
@@ -5000,29 +5009,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B48:B53"/>
-    <mergeCell ref="C48:C52"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D50:G52"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:G40"/>
-    <mergeCell ref="B34:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:G47"/>
-    <mergeCell ref="B42:C47"/>
-    <mergeCell ref="D12:G18"/>
-    <mergeCell ref="B13:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G25"/>
-    <mergeCell ref="B20:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G32"/>
-    <mergeCell ref="B27:C32"/>
-    <mergeCell ref="A1:A1048576"/>
-    <mergeCell ref="D1:G4"/>
     <mergeCell ref="H1:H1048576"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:C4"/>
@@ -5031,9 +5017,37 @@
     <mergeCell ref="D6:G11"/>
     <mergeCell ref="B7:C11"/>
     <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G32"/>
+    <mergeCell ref="B27:C32"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D50:G52"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="A1:A1048576"/>
+    <mergeCell ref="D1:G4"/>
+    <mergeCell ref="D12:G18"/>
+    <mergeCell ref="B13:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G25"/>
+    <mergeCell ref="B20:C25"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:G40"/>
+    <mergeCell ref="B34:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:G47"/>
+    <mergeCell ref="B42:C47"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C48:C52"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="43" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="51" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="50" max="16383" man="1"/>
+  </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>

</xml_diff>

<commit_message>
Attendance V2 new Code
</commit_message>
<xml_diff>
--- a/ProgramPartListWeb/Content/Uploads/PGFY-00031FORM_1.xlsx
+++ b/ProgramPartListWeb/Content/Uploads/PGFY-00031FORM_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.29.3.141\c$\inetpub\wwwroot\program-partlist\Content\Uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllSystems\P1saproject\ProgramPartListWeb\Content\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A318896-5644-4F7B-93C9-D94323367D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88229B65-36EF-43AC-A81F-6FFFE845C44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BFE99378-DD6B-4ABB-94CE-EAE1FDD2D083}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Production Patrol Inspection Report</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Date Conducted:</t>
+  </si>
+  <si>
+    <t>sdad</t>
+  </si>
+  <si>
+    <t>adad</t>
   </si>
 </sst>
 </file>
@@ -743,94 +749,61 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -862,14 +835,47 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4355,7 +4361,7 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="B7" sqref="B7:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4374,40 +4380,40 @@
     <row r="1" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="67"/>
     </row>
     <row r="2" spans="2:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="71"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="2:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -4417,473 +4423,477 @@
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60" t="s">
+      <c r="C6" s="44"/>
+      <c r="D6" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="65"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="50"/>
       <c r="I7" s="12"/>
     </row>
     <row r="8" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="65"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="50"/>
       <c r="I8" s="12"/>
     </row>
     <row r="9" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="65"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="65"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
       <c r="I10" s="12"/>
     </row>
     <row r="11" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="68"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53"/>
       <c r="I11" s="12"/>
     </row>
     <row r="12" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="45" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
       <c r="I12" s="12"/>
     </row>
     <row r="13" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
       <c r="I13" s="12"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
       <c r="I14" s="12"/>
     </row>
     <row r="15" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
       <c r="I15" s="12"/>
     </row>
     <row r="16" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
       <c r="I16" s="12"/>
     </row>
     <row r="17" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
       <c r="I17" s="12"/>
     </row>
     <row r="18" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="45" t="s">
+      <c r="C19" s="56"/>
+      <c r="D19" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
       <c r="I19" s="12"/>
     </row>
     <row r="20" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
       <c r="I20" s="12"/>
     </row>
     <row r="21" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
       <c r="I21" s="12"/>
     </row>
     <row r="22" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
       <c r="I24" s="12"/>
     </row>
     <row r="25" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
       <c r="I25" s="12"/>
     </row>
     <row r="26" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
       <c r="I26" s="12"/>
     </row>
     <row r="27" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="57"/>
       <c r="I27" s="12"/>
     </row>
     <row r="28" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="78"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
       <c r="I28" s="12"/>
     </row>
     <row r="29" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="78"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
       <c r="I29" s="12"/>
     </row>
     <row r="30" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="78"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
       <c r="I30" s="12"/>
     </row>
     <row r="31" spans="2:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="78"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
       <c r="I31" s="12"/>
     </row>
     <row r="32" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="78"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="45" t="s">
+      <c r="C33" s="56"/>
+      <c r="D33" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
       <c r="I33" s="12"/>
     </row>
     <row r="34" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
+      <c r="B34" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="72"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
       <c r="I34" s="12"/>
     </row>
     <row r="35" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="78"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
       <c r="I35" s="12"/>
     </row>
     <row r="36" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="78"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
       <c r="I36" s="12"/>
     </row>
     <row r="37" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
       <c r="I37" s="12"/>
     </row>
     <row r="38" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="78"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
       <c r="I38" s="12"/>
     </row>
     <row r="39" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="78"/>
-      <c r="C39" s="78"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="57"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="78"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
       <c r="I40" s="12"/>
     </row>
     <row r="41" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="48" t="s">
+      <c r="B41" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="45" t="s">
+      <c r="C41" s="56"/>
+      <c r="D41" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
       <c r="I41" s="12"/>
     </row>
     <row r="42" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="77"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
+      <c r="B42" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="72"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
       <c r="I42" s="12"/>
     </row>
     <row r="43" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="78"/>
-      <c r="C43" s="78"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
       <c r="I43" s="12"/>
     </row>
     <row r="44" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="78"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="78"/>
-      <c r="C45" s="78"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
       <c r="I45" s="12"/>
     </row>
     <row r="46" spans="2:9" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="78"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
       <c r="I46" s="12"/>
     </row>
     <row r="47" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="78"/>
-      <c r="C47" s="78"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
       <c r="I47" s="12"/>
     </row>
     <row r="48" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="50" t="s">
+      <c r="B48" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="53" t="s">
+      <c r="C48" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="69" t="s">
+      <c r="D48" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
-      <c r="G48" s="71"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="60"/>
       <c r="I48" s="12"/>
     </row>
     <row r="49" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="51"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="72" t="s">
+      <c r="B49" s="77"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="72"/>
-      <c r="F49" s="72"/>
-      <c r="G49" s="72"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
       <c r="I49" s="12"/>
     </row>
     <row r="50" spans="2:9" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="51"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="73" t="s">
+      <c r="B50" s="77"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="E50" s="73"/>
-      <c r="F50" s="73"/>
-      <c r="G50" s="73"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="62"/>
       <c r="I50" s="12"/>
     </row>
     <row r="51" spans="2:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="51"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="73"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="73"/>
-      <c r="G51" s="73"/>
+      <c r="B51" s="77"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
       <c r="I51" s="12"/>
     </row>
     <row r="52" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="51"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="73"/>
-      <c r="F52" s="73"/>
-      <c r="G52" s="73"/>
+      <c r="B52" s="77"/>
+      <c r="C52" s="79"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
       <c r="I52" s="12"/>
     </row>
     <row r="53" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="52"/>
+      <c r="B53" s="78"/>
       <c r="C53" s="35" t="s">
         <v>19</v>
       </c>
@@ -4902,10 +4912,10 @@
         <v>11</v>
       </c>
       <c r="C54" s="27"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="76"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="64"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="65"/>
       <c r="I54" s="19"/>
     </row>
     <row r="55" spans="2:9" ht="20.25" x14ac:dyDescent="0.25">
@@ -4994,8 +5004,8 @@
       <c r="D67" s="14"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="49"/>
-      <c r="C68" s="49"/>
+      <c r="B68" s="75"/>
+      <c r="C68" s="75"/>
       <c r="D68" s="14"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
@@ -5009,21 +5019,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H1:H1048576"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G11"/>
-    <mergeCell ref="B7:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:G32"/>
-    <mergeCell ref="B27:C32"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D50:G52"/>
-    <mergeCell ref="D54:G54"/>
     <mergeCell ref="A1:A1048576"/>
     <mergeCell ref="D1:G4"/>
     <mergeCell ref="D12:G18"/>
@@ -5040,6 +5035,21 @@
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="B48:B53"/>
     <mergeCell ref="C48:C52"/>
+    <mergeCell ref="H1:H1048576"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G11"/>
+    <mergeCell ref="B7:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:G32"/>
+    <mergeCell ref="B27:C32"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="D50:G52"/>
+    <mergeCell ref="D54:G54"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>